<commit_message>
fix post articulos y plantilla especiales
</commit_message>
<xml_diff>
--- a/public/plantillas/plantillaarticulos.xlsx
+++ b/public/plantillas/plantillaarticulos.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PlataformaComercial\public\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PlataformaComercial\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47A05FE-FDF7-46A4-BEF8-2C88CF16BDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1CFE228-0B28-4DA2-AF31-CE8E295299C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FE0B692A-4494-4C06-BB8C-F7171E0045E1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF114842-3951-4BE0-A4E4-59A6A41DE260}"/>
   </bookViews>
   <sheets>
-    <sheet name="Artículos" sheetId="1" r:id="rId1"/>
+    <sheet name="Articulos" sheetId="1" r:id="rId1"/>
+    <sheet name="Catalogo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,66 +34,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>E1</t>
+    <t>Campo</t>
   </si>
   <si>
-    <t>E2</t>
+    <t>Marca</t>
   </si>
   <si>
-    <t>E3</t>
+    <t>Valor</t>
   </si>
   <si>
-    <t>E4</t>
+    <t>Especial</t>
   </si>
   <si>
-    <t>E5</t>
+    <t>Proveedor</t>
   </si>
   <si>
-    <t>E6</t>
+    <t>Artículo</t>
   </si>
   <si>
-    <t>E7</t>
+    <t>CAMPO</t>
   </si>
   <si>
-    <t>E8</t>
-  </si>
-  <si>
-    <t>E9</t>
-  </si>
-  <si>
-    <t>E10</t>
-  </si>
-  <si>
-    <t>E11</t>
-  </si>
-  <si>
-    <t>E12</t>
-  </si>
-  <si>
-    <t>E13</t>
-  </si>
-  <si>
-    <t>E14</t>
-  </si>
-  <si>
-    <t>E15</t>
-  </si>
-  <si>
-    <t>E16</t>
-  </si>
-  <si>
-    <t>E17</t>
-  </si>
-  <si>
-    <t>E18</t>
-  </si>
-  <si>
-    <t>E19</t>
-  </si>
-  <si>
-    <t>E20</t>
+    <t>ESPECIAL</t>
   </si>
 </sst>
 </file>
@@ -115,13 +80,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,8 +101,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -143,59 +122,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -504,94 +507,207 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1464A2-6188-407B-9CF3-8DC11877231F}">
-  <dimension ref="A1:T1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA7BF0D-059A-433B-8F3D-5219192FD8F9}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="B2:E21"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{195D9FA7-2AC2-4733-8F85-F749F3FE72E5}">
+          <x14:formula1>
+            <xm:f>Catalogo!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2AA68EC2-9FC6-48D8-A9EF-63C4A252826C}">
+          <x14:formula1>
+            <xm:f>Catalogo!$B$2:$B$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0A13504-806C-4E33-B854-74B2FE57EFB3}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="3">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="3">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="3">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="3">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="3">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="3">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="3">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="3">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="3">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="3">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="3">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="3">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="3">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="3">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="3">
         <v>19</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="B22" s="3">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B2:B21">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C11">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D14">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E18">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
+  <mergeCells count="1">
+    <mergeCell ref="A6:A22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix caratula Comisiones 2.0
</commit_message>
<xml_diff>
--- a/public/plantillas/plantillaarticulos.xlsx
+++ b/public/plantillas/plantillaarticulos.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PlataformaComercial\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1CFE228-0B28-4DA2-AF31-CE8E295299C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9062B1-AE85-4F2A-9B9B-B10B089EFB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF114842-3951-4BE0-A4E4-59A6A41DE260}"/>
   </bookViews>
   <sheets>
     <sheet name="Articulos" sheetId="1" r:id="rId1"/>
-    <sheet name="Catalogo" sheetId="2" r:id="rId2"/>
+    <sheet name="Catalogo" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -51,13 +51,13 @@
     <t>Proveedor</t>
   </si>
   <si>
-    <t>Artículo</t>
-  </si>
-  <si>
     <t>CAMPO</t>
   </si>
   <si>
     <t>ESPECIAL</t>
+  </si>
+  <si>
+    <t>Articulo</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,17 +560,17 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -595,7 +595,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>

</xml_diff>